<commit_message>
Cleared some templates and etl_config.json
</commit_message>
<xml_diff>
--- a/queens/config/templates/dukes_ch_3.xlsx
+++ b/queens/config/templates/dukes_ch_3.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alessandro\PycharmProjects\uk_energy_data_api\data\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alessandro\AppData\Local\queens\queens\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FDD84F2-AFDC-40D7-8065-F613FB5ADE6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90CD8857-EB4A-4917-99B1-2BD72E93A2F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="3.1" sheetId="1" r:id="rId1"/>
@@ -2096,13 +2096,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G32"/>
   <sheetViews>
-    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
-    </sheetView>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="24.88671875" customWidth="1"/>
+    <col min="1" max="1" width="4.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
@@ -2467,7 +2470,7 @@
         <v>10</v>
       </c>
       <c r="F16" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="G16" t="s">
         <v>37</v>
@@ -2490,7 +2493,7 @@
         <v>10</v>
       </c>
       <c r="F17" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="G17" t="s">
         <v>37</v>
@@ -2513,7 +2516,7 @@
         <v>10</v>
       </c>
       <c r="F18" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="G18" t="s">
         <v>37</v>
@@ -2536,7 +2539,7 @@
         <v>10</v>
       </c>
       <c r="F19" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="G19" t="s">
         <v>37</v>
@@ -2559,7 +2562,7 @@
         <v>10</v>
       </c>
       <c r="F20" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="G20" t="s">
         <v>37</v>
@@ -2582,7 +2585,7 @@
         <v>10</v>
       </c>
       <c r="F21" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G21" t="s">
         <v>37</v>
@@ -2628,7 +2631,7 @@
         <v>20</v>
       </c>
       <c r="F23" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="G23" t="s">
         <v>37</v>
@@ -2651,7 +2654,7 @@
         <v>20</v>
       </c>
       <c r="F24" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G24" t="s">
         <v>37</v>
@@ -2674,7 +2677,7 @@
         <v>20</v>
       </c>
       <c r="F25" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="G25" t="s">
         <v>37</v>
@@ -2697,7 +2700,7 @@
         <v>20</v>
       </c>
       <c r="F26" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G26" t="s">
         <v>37</v>
@@ -2720,7 +2723,7 @@
         <v>20</v>
       </c>
       <c r="F27" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="G27" t="s">
         <v>37</v>
@@ -2743,7 +2746,7 @@
         <v>20</v>
       </c>
       <c r="F28" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="G28" t="s">
         <v>37</v>
@@ -2766,7 +2769,7 @@
         <v>20</v>
       </c>
       <c r="F29" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G29" t="s">
         <v>37</v>
@@ -2789,7 +2792,7 @@
         <v>20</v>
       </c>
       <c r="F30" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="G30" t="s">
         <v>37</v>
@@ -2812,7 +2815,7 @@
         <v>20</v>
       </c>
       <c r="F31" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G31" t="s">
         <v>37</v>
@@ -2850,11 +2853,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01B41B7A-2C3D-4E57-995C-29C4474E4F08}">
   <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="21.33203125" customWidth="1"/>
+    <col min="1" max="1" width="4.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
@@ -4128,7 +4139,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31027A86-7F1C-468A-AAAF-6A7BB0E2B479}">
   <dimension ref="A1:E44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+    <sheetView zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -4937,15 +4948,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11CC6622-CEAD-4D77-9284-6CE5F1058248}">
   <dimension ref="A1:G60"/>
   <sheetViews>
-    <sheetView topLeftCell="A32" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
-    </sheetView>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="13.5546875" customWidth="1"/>
-    <col min="5" max="5" width="13.33203125" customWidth="1"/>
-    <col min="6" max="6" width="17.33203125" customWidth="1"/>
+    <col min="1" max="1" width="4.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
@@ -5324,7 +5336,7 @@
         <v>10</v>
       </c>
       <c r="F16" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="G16" t="s">
         <v>37</v>
@@ -5348,7 +5360,7 @@
         <v>10</v>
       </c>
       <c r="F17" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="G17" t="s">
         <v>37</v>
@@ -5372,7 +5384,7 @@
         <v>10</v>
       </c>
       <c r="F18" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="G18" t="s">
         <v>37</v>
@@ -5396,7 +5408,7 @@
         <v>10</v>
       </c>
       <c r="F19" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="G19" t="s">
         <v>37</v>
@@ -5420,7 +5432,7 @@
         <v>10</v>
       </c>
       <c r="F20" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="G20" t="s">
         <v>37</v>
@@ -5444,7 +5456,7 @@
         <v>10</v>
       </c>
       <c r="F21" t="s">
-        <v>10</v>
+        <v>41</v>
       </c>
       <c r="G21" t="s">
         <v>37</v>
@@ -5492,7 +5504,7 @@
         <v>20</v>
       </c>
       <c r="F23" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="G23" t="s">
         <v>37</v>
@@ -5516,7 +5528,7 @@
         <v>20</v>
       </c>
       <c r="F24" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G24" t="s">
         <v>37</v>
@@ -5540,7 +5552,7 @@
         <v>20</v>
       </c>
       <c r="F25" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="G25" t="s">
         <v>37</v>
@@ -5564,7 +5576,7 @@
         <v>20</v>
       </c>
       <c r="F26" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G26" t="s">
         <v>37</v>
@@ -5588,7 +5600,7 @@
         <v>20</v>
       </c>
       <c r="F27" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="G27" t="s">
         <v>37</v>
@@ -5612,7 +5624,7 @@
         <v>20</v>
       </c>
       <c r="F28" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="G28" t="s">
         <v>37</v>
@@ -5636,7 +5648,7 @@
         <v>20</v>
       </c>
       <c r="F29" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G29" t="s">
         <v>37</v>
@@ -5660,7 +5672,7 @@
         <v>20</v>
       </c>
       <c r="F30" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="G30" t="s">
         <v>37</v>
@@ -5684,7 +5696,7 @@
         <v>20</v>
       </c>
       <c r="F31" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G31" t="s">
         <v>37</v>
@@ -6395,13 +6407,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08F518A5-C205-460E-8CCB-B23F7B1926B2}">
   <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="235" zoomScaleNormal="235" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
+    <sheetView showGridLines="0" zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="34.44140625" customWidth="1"/>
+    <col min="1" max="1" width="4.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="32.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
@@ -6978,7 +6992,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8037FEBA-A225-4140-8772-11AB115C1323}">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView zoomScale="220" zoomScaleNormal="220" workbookViewId="0"/>
+    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -7147,14 +7163,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BF98E2C-5059-45E8-A2AA-3D5FF548F21F}">
   <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
-    </sheetView>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="47" customWidth="1"/>
-    <col min="3" max="3" width="21" customWidth="1"/>
+    <col min="1" max="1" width="4.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="42.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
@@ -7731,13 +7749,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5D4C765-27B6-435A-8DF0-D533416DA58C}">
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
+    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="25.6640625" customWidth="1"/>
+    <col min="1" max="1" width="4.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
@@ -8142,13 +8162,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93AF7E55-CF5E-478B-AE82-46B1BDE0FD14}">
   <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
-    </sheetView>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="21.21875" customWidth="1"/>
+    <col min="1" max="1" width="4.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
@@ -8557,13 +8580,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B52A4735-F889-4EBB-BC98-D1B3E6568DE2}">
   <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
-    </sheetView>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="21.21875" customWidth="1"/>
+    <col min="1" max="1" width="4.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
@@ -8972,8 +8998,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{467EAA01-A872-4247-975B-CBD91630A6BD}">
   <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>